<commit_message>
before baking playcomebine scene
</commit_message>
<xml_diff>
--- a/Assets/8_Data/2_LevelData.xlsx
+++ b/Assets/8_Data/2_LevelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08E66C0-0FAE-4E58-BF90-7F03B636CEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Level_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data_Level_2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,92 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Có bật hồ hồi máu, không cần xếp hồ vào map
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+nhập tên prefab enemy tại
+\Resources\Enemy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nhập tên item tại resources/item folder
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,14 +201,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>GroundName</t>
   </si>
   <si>
-    <t>Ground_#_19</t>
-  </si>
-  <si>
     <t>HasRegen</t>
   </si>
   <si>
@@ -145,19 +227,91 @@
     <t>Enemy2_Level</t>
   </si>
   <si>
-    <t>#_1_Enemy_Skeleton</t>
-  </si>
-  <si>
-    <t>#_1_Enemy_Bat Lord</t>
-  </si>
-  <si>
     <t>ItemConsumable_EggFire</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green0</t>
+  </si>
+  <si>
+    <t>#_104_Creature_WolfPup_Fire</t>
+  </si>
+  <si>
+    <t>#_105_Creature_Sprout_Normal</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green1</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green4</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green6</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green8</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green3</t>
+  </si>
+  <si>
+    <t>#_104_Creature_WolfPup_Ice</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green2</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green5</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green7</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green9</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green10</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green11</t>
+  </si>
+  <si>
+    <t>#_7_Ground_Green12</t>
+  </si>
+  <si>
+    <t>#_105_Creature_Sprout_Fire</t>
+  </si>
+  <si>
+    <t>#_106_Creature_Fungi_Fire</t>
+  </si>
+  <si>
+    <t>#_108_Creature_Wolf_Normal</t>
+  </si>
+  <si>
+    <t>#_113_Creature_Cactus_Fire</t>
+  </si>
+  <si>
+    <t>#_102_Creature_Fledgling_Ice</t>
+  </si>
+  <si>
+    <t>#_108_Creature_Wolf_Ice</t>
+  </si>
+  <si>
+    <t>#_109_Creature_Bee_Normal</t>
+  </si>
+  <si>
+    <t>#_110_Creature_Bumble_Thunder</t>
+  </si>
+  <si>
+    <t>#_111_Creature_Angel_Normal</t>
+  </si>
+  <si>
+    <t>#_103_Creature_MushRoom_Ice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,54 +635,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="5" width="27.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="26.44140625" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
       <c r="H1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -537,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -546,10 +701,272 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>